<commit_message>
Changes for fan and lights.
</commit_message>
<xml_diff>
--- a/Marlin/3DR Calibration.xlsx
+++ b/Marlin/3DR Calibration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="24880" windowHeight="21040" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Positions" sheetId="1" r:id="rId1"/>
@@ -242,7 +242,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="76">
   <si>
     <t>DELTA_DIAGONAL_ROD</t>
   </si>
@@ -458,6 +458,18 @@
   </si>
   <si>
     <t>G4 200</t>
+  </si>
+  <si>
+    <t>M42 P7 S255</t>
+  </si>
+  <si>
+    <t>; Start LED light power</t>
+  </si>
+  <si>
+    <t>M42 P7 S0</t>
+  </si>
+  <si>
+    <t>; Turn off LED light power</t>
   </si>
 </sst>
 </file>
@@ -1468,6 +1480,9 @@
   </cellStyles>
   <dxfs count="46">
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
       <fill>
         <patternFill patternType="solid">
@@ -1485,6 +1500,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1497,6 +1515,9 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -1529,6 +1550,15 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1569,21 +1599,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
@@ -2057,9 +2072,6 @@
         <bottom/>
       </border>
     </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
@@ -2068,12 +2080,12 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B6:G12" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="44"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="43"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="42"/>
-    <tableColumn id="6" name="Z" dataDxfId="41" totalsRowDxfId="40" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="215.5" dataDxfId="39" totalsRowDxfId="38"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="37" totalsRowDxfId="36">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="45"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="44"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="43"/>
+    <tableColumn id="6" name="Z" dataDxfId="42" totalsRowDxfId="41" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="215.5" dataDxfId="40" totalsRowDxfId="39"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="37">
       <totalsRowFormula>"M666 X-"&amp;G9&amp;" Y-"&amp;G10&amp;" Z-"&amp;G11</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2084,12 +2096,12 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1425" displayName="Table1425" ref="B14:G20" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="35"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="34"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="33"/>
-    <tableColumn id="6" name="Z" dataDxfId="32" totalsRowDxfId="31" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="216.5" dataDxfId="30" totalsRowDxfId="29"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="28" totalsRowDxfId="27">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="36"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="35"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="34"/>
+    <tableColumn id="6" name="Z" dataDxfId="33" totalsRowDxfId="32" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="216.5" dataDxfId="31" totalsRowDxfId="30"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="28">
       <totalsRowFormula>"M666 X-"&amp;G17&amp;" Y-"&amp;G18&amp;" Z-"&amp;G19</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2100,12 +2112,12 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1427" displayName="Table1427" ref="I6:N12" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="26"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="25"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="24"/>
-    <tableColumn id="6" name="Z" dataDxfId="23" totalsRowDxfId="22" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="216.0" dataDxfId="21" totalsRowDxfId="20"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="19" totalsRowDxfId="18">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="27"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="26"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="25"/>
+    <tableColumn id="6" name="Z" dataDxfId="24" totalsRowDxfId="23" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="216.0" dataDxfId="22" totalsRowDxfId="21"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="19">
       <totalsRowFormula>"M666 X-"&amp;N9&amp;" Y-"&amp;N10&amp;" Z-"&amp;N11</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2116,12 +2128,12 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table14258" displayName="Table14258" ref="I14:N20" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="17"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="16"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="15"/>
-    <tableColumn id="6" name="Z" dataDxfId="14" totalsRowDxfId="13" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="217.0" dataDxfId="12" totalsRowDxfId="11"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="10" totalsRowDxfId="9">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="18"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="17"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="16"/>
+    <tableColumn id="6" name="Z" dataDxfId="15" totalsRowDxfId="14" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="217.0" dataDxfId="13" totalsRowDxfId="12"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
       <totalsRowFormula>"M666 X-"&amp;N17&amp;" Y-"&amp;N18&amp;" Z-"&amp;N19</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2132,12 +2144,12 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table142589" displayName="Table142589" ref="B22:G28" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="5"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="4"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="3"/>
-    <tableColumn id="6" name="Z" dataDxfId="8" totalsRowDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="217.5" dataDxfId="7" totalsRowDxfId="1"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="6" totalsRowDxfId="0">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="9"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="8"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="7"/>
+    <tableColumn id="6" name="Z" dataDxfId="6" totalsRowDxfId="5" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="217.5" dataDxfId="4" totalsRowDxfId="3"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="1">
       <totalsRowFormula>"M666 X-"&amp;G25&amp;" Y-"&amp;G26&amp;" Z-"&amp;G27</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2149,7 +2161,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:C16" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Parameter"/>
-    <tableColumn id="2" name="Value" dataDxfId="45"/>
+    <tableColumn id="2" name="Value" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -2479,7 +2491,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -3207,39 +3219,54 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C30"/>
+  <dimension ref="B2:H30"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="4.83203125" customWidth="1"/>
     <col min="2" max="2" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:3">
+    <row r="2" spans="2:8">
       <c r="B2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="2:3">
+    <row r="3" spans="2:8">
       <c r="B3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="5" spans="2:3">
+      <c r="G3" t="s">
+        <v>72</v>
+      </c>
+      <c r="H3" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8">
+      <c r="G4" t="s">
+        <v>74</v>
+      </c>
+      <c r="H4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8">
       <c r="B5" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="2:3">
+    <row r="6" spans="2:8">
       <c r="B6" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="2:3">
+    <row r="8" spans="2:8">
       <c r="B8" s="17" t="s">
         <v>42</v>
       </c>
@@ -3248,7 +3275,7 @@
         <v>G0 X0 Y0 Z10 E0</v>
       </c>
     </row>
-    <row r="9" spans="2:3">
+    <row r="9" spans="2:8">
       <c r="B9" s="17" t="s">
         <v>43</v>
       </c>
@@ -3257,7 +3284,7 @@
         <v>G0 X-99.46 Y-57.43 Z10 E0</v>
       </c>
     </row>
-    <row r="10" spans="2:3">
+    <row r="10" spans="2:8">
       <c r="B10" s="17" t="s">
         <v>44</v>
       </c>
@@ -3266,7 +3293,7 @@
         <v>G0 X99.46 Y-57.43 Z10 E0</v>
       </c>
     </row>
-    <row r="11" spans="2:3">
+    <row r="11" spans="2:8">
       <c r="B11" s="17" t="s">
         <v>45</v>
       </c>
@@ -3275,12 +3302,12 @@
         <v>G0 X0 Y114.85 Z10 E0</v>
       </c>
     </row>
-    <row r="13" spans="2:3">
+    <row r="13" spans="2:8">
       <c r="B13" s="19" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="16" spans="2:3">
+    <row r="16" spans="2:8">
       <c r="B16" t="s">
         <v>47</v>
       </c>

</xml_diff>

<commit_message>
Updated with heated bed PID test
</commit_message>
<xml_diff>
--- a/Marlin/3DR Calibration.xlsx
+++ b/Marlin/3DR Calibration.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24709"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24816"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="2080" yWindow="1800" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Positions" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,33 @@
         </r>
       </text>
     </comment>
+    <comment ref="I25" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Clockwise from extruder</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="B26" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>w/extruder</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I26" authorId="0">
       <text>
         <r>
           <rPr>
@@ -237,12 +263,25 @@
         </r>
       </text>
     </comment>
+    <comment ref="I27" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Calibri"/>
+            <family val="2"/>
+          </rPr>
+          <t>Counter clockwise from extruder</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="76">
   <si>
     <t>DELTA_DIAGONAL_ROD</t>
   </si>
@@ -548,9 +587,55 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="446">
+  <cellStyleXfs count="492">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1030,7 +1115,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="446">
+  <cellStyles count="492">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1254,6 +1339,29 @@
     <cellStyle name="Followed Hyperlink" xfId="441" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="443" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="445" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="447" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="449" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="451" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="453" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="455" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="457" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="459" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="461" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="463" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="465" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="467" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="469" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="471" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="473" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="475" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="477" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="479" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="481" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="483" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="485" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="487" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="489" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="491" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1476,12 +1584,32 @@
     <cellStyle name="Hyperlink" xfId="440" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="442" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="444" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="446" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="448" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="450" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="452" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="454" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="456" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="458" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="460" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="462" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="464" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="466" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="468" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="470" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="472" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="474" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="476" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="478" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="480" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="482" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="484" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="486" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="488" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="490" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="46">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
+  <dxfs count="55">
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
       <fill>
@@ -1500,9 +1628,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1515,9 +1640,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -1550,15 +1672,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1618,9 +1731,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1633,9 +1743,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -1668,15 +1775,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1736,9 +1834,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1751,9 +1846,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -1786,15 +1878,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1854,9 +1937,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1869,9 +1949,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -1904,15 +1981,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1972,9 +2040,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1987,9 +2052,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -2022,15 +2084,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2071,6 +2124,202 @@
         <top/>
         <bottom/>
       </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -2080,12 +2329,12 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B6:G12" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="45"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="44"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="43"/>
-    <tableColumn id="6" name="Z" dataDxfId="42" totalsRowDxfId="41" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="215.5" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="37">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="4"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="3"/>
+    <tableColumn id="6" name="Z" dataDxfId="54" totalsRowDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="215.5" dataDxfId="53" totalsRowDxfId="1"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="52" totalsRowDxfId="0">
       <totalsRowFormula>"M666 X-"&amp;G9&amp;" Y-"&amp;G10&amp;" Z-"&amp;G11</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2096,12 +2345,12 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1425" displayName="Table1425" ref="B14:G20" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="36"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="35"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="34"/>
-    <tableColumn id="6" name="Z" dataDxfId="33" totalsRowDxfId="32" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="216.5" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="35"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="34"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="33"/>
+    <tableColumn id="6" name="Z" dataDxfId="51" totalsRowDxfId="32" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="216.5" dataDxfId="50" totalsRowDxfId="31"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="49" totalsRowDxfId="30">
       <totalsRowFormula>"M666 X-"&amp;G17&amp;" Y-"&amp;G18&amp;" Z-"&amp;G19</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2112,12 +2361,12 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1427" displayName="Table1427" ref="I6:N12" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="27"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="26"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="25"/>
-    <tableColumn id="6" name="Z" dataDxfId="24" totalsRowDxfId="23" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="216.0" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="19">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="11"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="10"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="9"/>
+    <tableColumn id="6" name="Z" dataDxfId="48" totalsRowDxfId="8" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="216.0" dataDxfId="47" totalsRowDxfId="7"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="46" totalsRowDxfId="6">
       <totalsRowFormula>"M666 X-"&amp;N9&amp;" Y-"&amp;N10&amp;" Z-"&amp;N11</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2128,12 +2377,12 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table14258" displayName="Table14258" ref="I14:N20" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="18"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="17"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="16"/>
-    <tableColumn id="6" name="Z" dataDxfId="15" totalsRowDxfId="14" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="217.0" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="23"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="22"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="21"/>
+    <tableColumn id="6" name="Z" dataDxfId="45" totalsRowDxfId="20" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="217.0" dataDxfId="44" totalsRowDxfId="19"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="43" totalsRowDxfId="18">
       <totalsRowFormula>"M666 X-"&amp;N17&amp;" Y-"&amp;N18&amp;" Z-"&amp;N19</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2144,12 +2393,12 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table142589" displayName="Table142589" ref="B22:G28" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="9"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="8"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="7"/>
-    <tableColumn id="6" name="Z" dataDxfId="6" totalsRowDxfId="5" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="217.5" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="1">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="29"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="28"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="27"/>
+    <tableColumn id="6" name="Z" dataDxfId="42" totalsRowDxfId="26" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="217.5" dataDxfId="41" totalsRowDxfId="25"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="40" totalsRowDxfId="24">
       <totalsRowFormula>"M666 X-"&amp;G25&amp;" Y-"&amp;G26&amp;" Z-"&amp;G27</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -2158,10 +2407,26 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1425892" displayName="Table1425892" ref="I22:N28" totalsRowCount="1">
+  <tableColumns count="6">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="17"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="16"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="15"/>
+    <tableColumn id="6" name="Z" dataDxfId="38" totalsRowDxfId="14" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="217.5" dataDxfId="37" totalsRowDxfId="13"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="36" totalsRowDxfId="12">
+      <totalsRowFormula>"M666 X-"&amp;N25&amp;" Y-"&amp;N26&amp;" Z-"&amp;N27</totalsRowFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
+</table>
+</file>
+
+<file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:C16" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Parameter"/>
-    <tableColumn id="2" name="Value" dataDxfId="0"/>
+    <tableColumn id="2" name="Value" dataDxfId="39"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -2491,8 +2756,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A4" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2617,7 +2882,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
       <c r="F7" s="6">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G7" s="6">
         <f>MIN(F9:F11)</f>
@@ -2629,12 +2894,10 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="6">
-        <v>117</v>
-      </c>
+      <c r="M7" s="6"/>
       <c r="N7" s="6">
         <f>MIN(M9:M11)</f>
-        <v>116.2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:14">
@@ -2648,11 +2911,11 @@
         <v>0</v>
       </c>
       <c r="E8" s="5">
-        <v>1.2</v>
+        <v>3.2</v>
       </c>
       <c r="F8" s="6">
         <f>F$7-Table14[[#This Row],[Z]]</f>
-        <v>115.8</v>
+        <v>116.8</v>
       </c>
       <c r="G8"/>
       <c r="I8" t="s">
@@ -2664,12 +2927,10 @@
       <c r="K8" s="5">
         <v>0</v>
       </c>
-      <c r="L8" s="5">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="L8" s="5"/>
       <c r="M8" s="6">
         <f>M$7-Table1427[[#This Row],[Z]]</f>
-        <v>115.9</v>
+        <v>0</v>
       </c>
       <c r="N8"/>
     </row>
@@ -2684,15 +2945,15 @@
         <v>-57.4</v>
       </c>
       <c r="E9" s="5">
-        <v>0.9</v>
+        <v>3.2</v>
       </c>
       <c r="F9" s="6">
         <f>F$7-Table14[[#This Row],[Z]]</f>
-        <v>116.1</v>
+        <v>116.8</v>
       </c>
       <c r="G9" s="6">
         <f>ROUNDUP(MAX(E$9:E$11),1)-Table14[[#This Row],[Z]]</f>
-        <v>0</v>
+        <v>0.69999999999999973</v>
       </c>
       <c r="I9" t="s">
         <v>7</v>
@@ -2703,12 +2964,10 @@
       <c r="K9" s="5">
         <v>-57.4</v>
       </c>
-      <c r="L9" s="5">
-        <v>0.8</v>
-      </c>
+      <c r="L9" s="5"/>
       <c r="M9" s="6">
         <f>M$7-Table1427[[#This Row],[Z]]</f>
-        <v>116.2</v>
+        <v>0</v>
       </c>
       <c r="N9" s="6">
         <f>ROUNDUP(MAX(L$9:L$11),1)-Table1427[[#This Row],[Z]]</f>
@@ -2726,15 +2985,15 @@
         <v>-57.4</v>
       </c>
       <c r="E10" s="5">
-        <v>0.6</v>
+        <v>3.9</v>
       </c>
       <c r="F10" s="6">
         <f>F$7-Table14[[#This Row],[Z]]</f>
-        <v>116.4</v>
+        <v>116.1</v>
       </c>
       <c r="G10" s="6">
         <f>ROUNDUP(MAX(E$17:E$19),1)-Table14[[#This Row],[Z]]</f>
-        <v>0.4</v>
+        <v>-3.9</v>
       </c>
       <c r="I10" t="s">
         <v>8</v>
@@ -2745,12 +3004,10 @@
       <c r="K10" s="5">
         <v>-57.4</v>
       </c>
-      <c r="L10" s="5">
-        <v>0.8</v>
-      </c>
+      <c r="L10" s="5"/>
       <c r="M10" s="6">
         <f>M$7-Table1427[[#This Row],[Z]]</f>
-        <v>116.2</v>
+        <v>0</v>
       </c>
       <c r="N10" s="6">
         <f>ROUNDUP(MAX(L$9:L$11),1)-Table1427[[#This Row],[Z]]</f>
@@ -2768,15 +3025,15 @@
         <v>114.8</v>
       </c>
       <c r="E11" s="5">
-        <v>0.6</v>
+        <v>1.4</v>
       </c>
       <c r="F11" s="6">
         <f>F$7-Table14[[#This Row],[Z]]</f>
-        <v>116.4</v>
+        <v>118.6</v>
       </c>
       <c r="G11" s="6">
         <f>ROUNDUP(MAX(E$17:E$19),1)-Table14[[#This Row],[Z]]</f>
-        <v>0.4</v>
+        <v>-1.4</v>
       </c>
       <c r="I11" t="s">
         <v>9</v>
@@ -2787,12 +3044,10 @@
       <c r="K11" s="5">
         <v>114.8</v>
       </c>
-      <c r="L11" s="5">
-        <v>0.8</v>
-      </c>
+      <c r="L11" s="5"/>
       <c r="M11" s="6">
         <f>M$7-Table1427[[#This Row],[Z]]</f>
-        <v>116.2</v>
+        <v>0</v>
       </c>
       <c r="N11" s="6">
         <f>ROUNDUP(MAX(L$9:L$11),1)-Table1427[[#This Row],[Z]]</f>
@@ -2807,7 +3062,7 @@
       <c r="F12" s="13"/>
       <c r="G12" s="14" t="str">
         <f>"M666 X-"&amp;G9&amp;" Y-"&amp;G10&amp;" Z-"&amp;G11</f>
-        <v>M666 X-0 Y-0.4 Z-0.4</v>
+        <v>M666 X-0.7 Y--3.9 Z--1.4</v>
       </c>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
@@ -2864,12 +3119,10 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="6">
-        <v>117</v>
-      </c>
+      <c r="F15" s="6"/>
       <c r="G15" s="6">
         <f>MIN(F17:F19)</f>
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="I15" t="s">
         <v>5</v>
@@ -2877,12 +3130,10 @@
       <c r="J15" s="4"/>
       <c r="K15" s="4"/>
       <c r="L15" s="4"/>
-      <c r="M15" s="6">
-        <v>117</v>
-      </c>
+      <c r="M15" s="6"/>
       <c r="N15" s="6">
         <f>MIN(M17:M19)</f>
-        <v>115.9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="2:14">
@@ -2895,12 +3146,10 @@
       <c r="D16" s="5">
         <v>0</v>
       </c>
-      <c r="E16" s="5">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="E16" s="5"/>
       <c r="F16" s="6">
         <f>F$15-Table1425[[#This Row],[Z]]</f>
-        <v>115.9</v>
+        <v>0</v>
       </c>
       <c r="G16"/>
       <c r="I16" t="s">
@@ -2912,12 +3161,10 @@
       <c r="K16" s="5">
         <v>0</v>
       </c>
-      <c r="L16" s="5">
-        <v>1.2</v>
-      </c>
+      <c r="L16" s="5"/>
       <c r="M16" s="6">
         <f>M$15-Table14258[[#This Row],[Z]]</f>
-        <v>115.8</v>
+        <v>0</v>
       </c>
       <c r="N16"/>
     </row>
@@ -2931,12 +3178,10 @@
       <c r="D17" s="5">
         <v>-57.4</v>
       </c>
-      <c r="E17" s="5">
-        <v>1</v>
-      </c>
+      <c r="E17" s="5"/>
       <c r="F17" s="6">
         <f>F$15-Table1425[[#This Row],[Z]]</f>
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="G17" s="6">
         <f>ROUNDUP(MAX(E$17:E$19),1)-Table1425[[#This Row],[Z]]</f>
@@ -2951,12 +3196,10 @@
       <c r="K17" s="5">
         <v>-57.4</v>
       </c>
-      <c r="L17" s="5">
-        <v>1.1000000000000001</v>
-      </c>
+      <c r="L17" s="5"/>
       <c r="M17" s="6">
         <f>M$15-Table14258[[#This Row],[Z]]</f>
-        <v>115.9</v>
+        <v>0</v>
       </c>
       <c r="N17" s="6">
         <f>ROUNDUP(MAX(L$17:L$19),1)-Table14258[[#This Row],[Z]]</f>
@@ -2973,16 +3216,14 @@
       <c r="D18" s="5">
         <v>-57.4</v>
       </c>
-      <c r="E18" s="5">
-        <v>0.9</v>
-      </c>
+      <c r="E18" s="5"/>
       <c r="F18" s="6">
         <f>F$15-Table1425[[#This Row],[Z]]</f>
-        <v>116.1</v>
+        <v>0</v>
       </c>
       <c r="G18" s="6">
         <f>ROUNDUP(MAX(E$17:E$19),1)-Table1425[[#This Row],[Z]]</f>
-        <v>9.9999999999999978E-2</v>
+        <v>0</v>
       </c>
       <c r="I18" t="s">
         <v>8</v>
@@ -2993,16 +3234,14 @@
       <c r="K18" s="5">
         <v>-57.4</v>
       </c>
-      <c r="L18" s="5">
-        <v>1</v>
-      </c>
+      <c r="L18" s="5"/>
       <c r="M18" s="6">
         <f>M$15-Table14258[[#This Row],[Z]]</f>
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="N18" s="6">
         <f>ROUNDUP(MAX(L$17:L$19),1)-Table14258[[#This Row],[Z]]</f>
-        <v>0.10000000000000009</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:14">
@@ -3015,16 +3254,14 @@
       <c r="D19" s="5">
         <v>114.8</v>
       </c>
-      <c r="E19" s="5">
-        <v>0.9</v>
-      </c>
+      <c r="E19" s="5"/>
       <c r="F19" s="6">
         <f>F$15-Table1425[[#This Row],[Z]]</f>
-        <v>116.1</v>
+        <v>0</v>
       </c>
       <c r="G19" s="6">
         <f>ROUNDUP(MAX(E$17:E$19),1)-Table1425[[#This Row],[Z]]</f>
-        <v>9.9999999999999978E-2</v>
+        <v>0</v>
       </c>
       <c r="I19" t="s">
         <v>9</v>
@@ -3035,16 +3272,14 @@
       <c r="K19" s="5">
         <v>114.8</v>
       </c>
-      <c r="L19" s="5">
-        <v>1</v>
-      </c>
+      <c r="L19" s="5"/>
       <c r="M19" s="6">
         <f>M$15-Table14258[[#This Row],[Z]]</f>
-        <v>116</v>
+        <v>0</v>
       </c>
       <c r="N19" s="6">
         <f>ROUNDUP(MAX(L$17:L$19),1)-Table14258[[#This Row],[Z]]</f>
-        <v>0.10000000000000009</v>
+        <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:14">
@@ -3055,7 +3290,7 @@
       <c r="F20" s="13"/>
       <c r="G20" s="14" t="str">
         <f>"M666 X-"&amp;G17&amp;" Y-"&amp;G18&amp;" Z-"&amp;G19</f>
-        <v>M666 X-0 Y-0.1 Z-0.1</v>
+        <v>M666 X-0 Y-0 Z-0</v>
       </c>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -3064,7 +3299,7 @@
       <c r="M20" s="13"/>
       <c r="N20" s="14" t="str">
         <f>"M666 X-"&amp;N17&amp;" Y-"&amp;N18&amp;" Z-"&amp;N19</f>
-        <v>M666 X-0 Y-0.1 Z-0.1</v>
+        <v>M666 X-0 Y-0 Z-0</v>
       </c>
     </row>
     <row r="22" spans="2:14">
@@ -3084,6 +3319,24 @@
         <v>37</v>
       </c>
       <c r="G22" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I22" t="s">
+        <v>0</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="M22" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="N22" s="1" t="s">
         <v>27</v>
       </c>
     </row>
@@ -3094,12 +3347,21 @@
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
       <c r="E23" s="4"/>
-      <c r="F23" s="6">
-        <v>116.1</v>
-      </c>
+      <c r="F23" s="6"/>
       <c r="G23" s="6">
         <f>MIN(F25:F27)</f>
-        <v>116.1</v>
+        <v>0</v>
+      </c>
+      <c r="I23" t="s">
+        <v>5</v>
+      </c>
+      <c r="J23" s="4"/>
+      <c r="K23" s="4"/>
+      <c r="L23" s="4"/>
+      <c r="M23" s="6"/>
+      <c r="N23" s="6">
+        <f>MIN(M25:M27)</f>
+        <v>0</v>
       </c>
     </row>
     <row r="24" spans="2:14">
@@ -3112,14 +3374,27 @@
       <c r="D24" s="5">
         <v>0</v>
       </c>
-      <c r="E24" s="5">
-        <v>0</v>
-      </c>
+      <c r="E24" s="5"/>
       <c r="F24" s="6">
         <f>F$23-Table142589[[#This Row],[Z]]</f>
-        <v>116.1</v>
+        <v>0</v>
       </c>
       <c r="G24"/>
+      <c r="I24" t="s">
+        <v>6</v>
+      </c>
+      <c r="J24" s="5">
+        <v>0</v>
+      </c>
+      <c r="K24" s="5">
+        <v>0</v>
+      </c>
+      <c r="L24" s="5"/>
+      <c r="M24" s="6">
+        <f>M$23-Table1425892[[#This Row],[Z]]</f>
+        <v>0</v>
+      </c>
+      <c r="N24"/>
     </row>
     <row r="25" spans="2:14">
       <c r="B25" t="s">
@@ -3131,15 +3406,31 @@
       <c r="D25" s="5">
         <v>-57.4</v>
       </c>
-      <c r="E25" s="5">
-        <v>0</v>
-      </c>
+      <c r="E25" s="5"/>
       <c r="F25" s="6">
         <f>F$23-Table142589[[#This Row],[Z]]</f>
-        <v>116.1</v>
+        <v>0</v>
       </c>
       <c r="G25" s="6">
         <f>MAX(E$25:E$27)-Table142589[[#This Row],[Z]]</f>
+        <v>0</v>
+      </c>
+      <c r="I25" t="s">
+        <v>7</v>
+      </c>
+      <c r="J25" s="5">
+        <v>-99.4</v>
+      </c>
+      <c r="K25" s="5">
+        <v>-57.4</v>
+      </c>
+      <c r="L25" s="5"/>
+      <c r="M25" s="6">
+        <f>M$23-Table1425892[[#This Row],[Z]]</f>
+        <v>0</v>
+      </c>
+      <c r="N25" s="6">
+        <f>MAX(L$25:L$27)-Table1425892[[#This Row],[Z]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3153,15 +3444,31 @@
       <c r="D26" s="5">
         <v>-57.4</v>
       </c>
-      <c r="E26" s="5">
-        <v>0</v>
-      </c>
+      <c r="E26" s="5"/>
       <c r="F26" s="6">
         <f>F$23-Table142589[[#This Row],[Z]]</f>
-        <v>116.1</v>
+        <v>0</v>
       </c>
       <c r="G26" s="6">
         <f>MAX(E$25:E$27)-Table142589[[#This Row],[Z]]</f>
+        <v>0</v>
+      </c>
+      <c r="I26" t="s">
+        <v>8</v>
+      </c>
+      <c r="J26" s="5">
+        <v>99.4</v>
+      </c>
+      <c r="K26" s="5">
+        <v>-57.4</v>
+      </c>
+      <c r="L26" s="5"/>
+      <c r="M26" s="6">
+        <f>M$23-Table1425892[[#This Row],[Z]]</f>
+        <v>0</v>
+      </c>
+      <c r="N26" s="6">
+        <f>MAX(L$25:L$27)-Table1425892[[#This Row],[Z]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3175,15 +3482,31 @@
       <c r="D27" s="5">
         <v>114.8</v>
       </c>
-      <c r="E27" s="5">
-        <v>0</v>
-      </c>
+      <c r="E27" s="5"/>
       <c r="F27" s="6">
         <f>F$23-Table142589[[#This Row],[Z]]</f>
-        <v>116.1</v>
+        <v>0</v>
       </c>
       <c r="G27" s="6">
         <f>MAX(E$25:E$27)-Table142589[[#This Row],[Z]]</f>
+        <v>0</v>
+      </c>
+      <c r="I27" t="s">
+        <v>9</v>
+      </c>
+      <c r="J27" s="5">
+        <v>0</v>
+      </c>
+      <c r="K27" s="5">
+        <v>114.8</v>
+      </c>
+      <c r="L27" s="5"/>
+      <c r="M27" s="6">
+        <f>M$23-Table1425892[[#This Row],[Z]]</f>
+        <v>0</v>
+      </c>
+      <c r="N27" s="6">
+        <f>MAX(L$25:L$27)-Table1425892[[#This Row],[Z]]</f>
         <v>0</v>
       </c>
     </row>
@@ -3197,17 +3520,27 @@
         <f>"M666 X-"&amp;G25&amp;" Y-"&amp;G26&amp;" Z-"&amp;G27</f>
         <v>M666 X-0 Y-0 Z-0</v>
       </c>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="12"/>
+      <c r="L28" s="16"/>
+      <c r="M28" s="13"/>
+      <c r="N28" s="14" t="str">
+        <f>"M666 X-"&amp;N25&amp;" Y-"&amp;N26&amp;" Z-"&amp;N27</f>
+        <v>M666 X-0 Y-0 Z-0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
-  <tableParts count="5">
+  <tableParts count="6">
     <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
     <tablePart r:id="rId6"/>
+    <tablePart r:id="rId7"/>
   </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -3221,7 +3554,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:H30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Callibration as of 11/05/2014
</commit_message>
<xml_diff>
--- a/Marlin/3DR Calibration.xlsx
+++ b/Marlin/3DR Calibration.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32020" windowHeight="21160" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19180" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Positions - Heated" sheetId="4" r:id="rId1"/>
@@ -26,6 +26,7 @@
     <definedName name="DELTA_TOWER2_Y">Parameters!$C$16</definedName>
     <definedName name="DELTA_TOWER3_X">Parameters!$C$13</definedName>
     <definedName name="DELTA_TOWER3_Y">Parameters!$C$14</definedName>
+    <definedName name="Height">Parameters!$E$7</definedName>
     <definedName name="SIN_60">Parameters!$C$9</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
@@ -526,7 +527,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="69">
   <si>
     <t>DELTA_DIAGONAL_ROD</t>
   </si>
@@ -727,6 +728,12 @@
   </si>
   <si>
     <t>M42 P7 S255 ; turn on the LEDs to high</t>
+  </si>
+  <si>
+    <t>Height</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -811,9 +818,289 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="506">
+  <cellStyleXfs count="786">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1354,7 +1641,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="506">
+  <cellStyles count="786">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -1608,6 +1895,146 @@
     <cellStyle name="Followed Hyperlink" xfId="501" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="503" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="505" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="507" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="509" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="511" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="513" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="515" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="517" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="519" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="521" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="523" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="525" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="527" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="529" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="531" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="533" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="535" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="537" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="539" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="541" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="543" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="545" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="547" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="549" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="551" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="553" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="555" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="557" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="559" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="561" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="563" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="565" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="567" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="569" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="571" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="573" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="575" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="577" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="579" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="581" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="583" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="585" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="587" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="589" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="591" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="593" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="595" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="597" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="599" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="601" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="603" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="605" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="607" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="609" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="611" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="613" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="615" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="617" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="619" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="621" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="623" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="625" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="627" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="629" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="631" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="633" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="635" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="637" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="639" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="641" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="643" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="645" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="647" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="649" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="651" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="653" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="655" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="657" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="659" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="661" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="663" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="665" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="667" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="669" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="671" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="673" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="675" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="677" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="679" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="681" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="683" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="685" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="687" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="689" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="691" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="693" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="695" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="697" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="699" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="701" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="703" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="705" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="707" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="709" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="711" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="713" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="715" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="717" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="719" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="721" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="723" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="725" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="727" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="729" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="731" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="733" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="735" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="737" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="739" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="741" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="743" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="745" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="747" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="749" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="751" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="753" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="755" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="757" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="759" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="761" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="763" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="765" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="767" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="769" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="771" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="773" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="775" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="777" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="779" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="781" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="783" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="785" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -1860,13 +2287,150 @@
     <cellStyle name="Hyperlink" xfId="500" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="502" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="504" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="506" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="508" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="510" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="512" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="514" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="516" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="518" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="520" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="522" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="524" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="526" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="528" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="530" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="532" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="534" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="536" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="538" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="540" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="542" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="544" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="546" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="548" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="550" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="552" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="554" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="556" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="558" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="560" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="562" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="564" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="566" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="568" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="570" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="572" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="574" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="576" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="578" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="580" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="582" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="584" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="586" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="588" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="590" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="592" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="594" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="596" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="598" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="600" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="602" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="604" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="606" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="608" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="610" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="612" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="614" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="616" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="618" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="620" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="622" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="624" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="626" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="628" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="630" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="632" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="634" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="636" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="638" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="640" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="642" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="644" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="646" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="648" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="650" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="652" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="654" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="656" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="658" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="660" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="662" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="664" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="666" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="668" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="670" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="672" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="674" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="676" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="678" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="680" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="682" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="684" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="686" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="688" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="690" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="692" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="694" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="696" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="698" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="700" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="702" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="704" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="706" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="708" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="710" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="712" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="714" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="716" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="718" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="720" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="722" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="724" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="726" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="728" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="730" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="732" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="734" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="736" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="738" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="740" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="742" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="744" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="746" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="748" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="750" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="752" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="754" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="756" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="758" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="760" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="762" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="764" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="766" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="768" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="770" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="772" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="774" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="776" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="778" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="780" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="782" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="784" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="109">
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
       <fill>
         <patternFill patternType="solid">
@@ -1884,24 +2448,18 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -1934,15 +2492,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2002,24 +2551,18 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2052,15 +2595,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2120,24 +2654,18 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2170,15 +2698,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2238,24 +2757,18 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2288,15 +2801,6 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2356,24 +2860,18 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -2406,55 +2904,49 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
@@ -3166,6 +3658,81 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3296,7 +3863,7 @@
     <tableColumn id="6" name="Z" dataDxfId="105" totalsRowDxfId="104" dataCellStyle="Comma"/>
     <tableColumn id="7" name="215.5" dataDxfId="103" totalsRowDxfId="102"/>
     <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="101" totalsRowDxfId="100">
-      <totalsRowFormula>"M666 X-"&amp;G9&amp;" Y-"&amp;G10&amp;" Z-"&amp;G11</totalsRowFormula>
+      <totalsRowFormula>"M666 X-"&amp;ROUND(G9,2)&amp;" Y-"&amp;ROUND(G10,2)&amp;" Z-"&amp;ROUND(G11,2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
@@ -3306,12 +3873,12 @@
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table14258" displayName="Table14258" ref="I14:N20" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="27"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="26"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="25"/>
-    <tableColumn id="6" name="Z" dataDxfId="24" totalsRowDxfId="23" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="217.0" dataDxfId="22" totalsRowDxfId="21"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="20" totalsRowDxfId="19">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="57"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="56"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="55"/>
+    <tableColumn id="6" name="Z" dataDxfId="54" totalsRowDxfId="53" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="217.0" dataDxfId="52" totalsRowDxfId="51"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="50" totalsRowDxfId="49">
       <totalsRowFormula>"M666 X-"&amp;N17&amp;" Y-"&amp;N18&amp;" Z-"&amp;N19</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3322,12 +3889,12 @@
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table142589" displayName="Table142589" ref="B22:G28" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="18"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="17"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="16"/>
-    <tableColumn id="6" name="Z" dataDxfId="15" totalsRowDxfId="14" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="217.5" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="11" totalsRowDxfId="10">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="48"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="47"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="46"/>
+    <tableColumn id="6" name="Z" dataDxfId="45" totalsRowDxfId="44" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="217.5" dataDxfId="43" totalsRowDxfId="42"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="40">
       <totalsRowFormula>"M666 X-"&amp;G25&amp;" Y-"&amp;G26&amp;" Z-"&amp;G27</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3338,12 +3905,12 @@
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1425892" displayName="Table1425892" ref="I22:N28" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="9"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="8"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="7"/>
-    <tableColumn id="6" name="Z" dataDxfId="6" totalsRowDxfId="5" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="217.5" dataDxfId="4" totalsRowDxfId="3"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="2" totalsRowDxfId="1">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="39"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="38"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="37"/>
+    <tableColumn id="6" name="Z" dataDxfId="36" totalsRowDxfId="35" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="217.5" dataDxfId="34" totalsRowDxfId="33"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="31">
       <totalsRowFormula>"M666 X-"&amp;N25&amp;" Y-"&amp;N26&amp;" Z-"&amp;N27</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3355,7 +3922,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:C16" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Parameter"/>
-    <tableColumn id="2" name="Value" dataDxfId="0"/>
+    <tableColumn id="2" name="Value" dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -3364,13 +3931,13 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table142510" displayName="Table142510" ref="B14:G20" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="99"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="98"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="97"/>
-    <tableColumn id="6" name="Z" dataDxfId="96" totalsRowDxfId="95" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="216.5" dataDxfId="94" totalsRowDxfId="93"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="92" totalsRowDxfId="91">
-      <totalsRowFormula>"M666 X-"&amp;G17&amp;" Y-"&amp;G18&amp;" Z-"&amp;G19</totalsRowFormula>
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="23"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="22"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="21"/>
+    <tableColumn id="6" name="Z" dataDxfId="99" totalsRowDxfId="20" dataCellStyle="Comma"/>
+    <tableColumn id="7" name=" " dataDxfId="98" totalsRowDxfId="19"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="97" totalsRowDxfId="18">
+      <totalsRowFormula>"M666 X-"&amp;ROUND(G17,2)&amp;" Y-"&amp;ROUND(G18,2)&amp;" Z-"&amp;ROUND(G19,2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
@@ -3380,13 +3947,13 @@
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="10" name="Table142711" displayName="Table142711" ref="I6:N12" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="90"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="89"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="88"/>
-    <tableColumn id="6" name="Z" dataDxfId="87" totalsRowDxfId="86" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="216.0" dataDxfId="85" totalsRowDxfId="84"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="83" totalsRowDxfId="82">
-      <totalsRowFormula>"M666 X-"&amp;N9&amp;" Y-"&amp;N10&amp;" Z-"&amp;N11</totalsRowFormula>
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="5"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="4"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="3"/>
+    <tableColumn id="6" name="Z" dataDxfId="96" totalsRowDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="7" name=" " dataDxfId="95" totalsRowDxfId="1"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="94" totalsRowDxfId="0">
+      <totalsRowFormula>"M666 X-"&amp;ROUND(N9,2)&amp;" Y-"&amp;ROUND(N10,2)&amp;" Z-"&amp;ROUND(N11,2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
@@ -3396,13 +3963,13 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1425812" displayName="Table1425812" ref="I14:N20" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="81"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="80"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="79"/>
-    <tableColumn id="6" name="Z" dataDxfId="78" totalsRowDxfId="77" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="217.0" dataDxfId="76" totalsRowDxfId="75"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="74" totalsRowDxfId="73">
-      <totalsRowFormula>"M666 X-"&amp;N17&amp;" Y-"&amp;N18&amp;" Z-"&amp;N19</totalsRowFormula>
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="29"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="28"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="27"/>
+    <tableColumn id="6" name="Z" dataDxfId="93" totalsRowDxfId="26" dataCellStyle="Comma"/>
+    <tableColumn id="7" name=" " dataDxfId="92" totalsRowDxfId="25"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="91" totalsRowDxfId="24">
+      <totalsRowFormula>"M666 X-"&amp;ROUND(N17,2)&amp;" Y-"&amp;ROUND(N18,2)&amp;" Z-"&amp;ROUND(N19,2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
@@ -3412,13 +3979,13 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table14258913" displayName="Table14258913" ref="B22:G28" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="72"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="71"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="70"/>
-    <tableColumn id="6" name="Z" dataDxfId="69" totalsRowDxfId="68" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="217.5" dataDxfId="67" totalsRowDxfId="66"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="65" totalsRowDxfId="64">
-      <totalsRowFormula>"M666 X-"&amp;G25&amp;" Y-"&amp;G26&amp;" Z-"&amp;G27</totalsRowFormula>
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="17"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="16"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="15"/>
+    <tableColumn id="6" name="Z" dataDxfId="90" totalsRowDxfId="14" dataCellStyle="Comma"/>
+    <tableColumn id="7" name=" " dataDxfId="89" totalsRowDxfId="13"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="88" totalsRowDxfId="12">
+      <totalsRowFormula>"M666 X-"&amp;ROUND(G25,2)&amp;" Y-"&amp;ROUND(G26,2)&amp;" Z-"&amp;ROUND(G27,2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
@@ -3428,13 +3995,13 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table142589214" displayName="Table142589214" ref="I22:N28" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="63"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="62"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="61"/>
-    <tableColumn id="6" name="Z" dataDxfId="60" totalsRowDxfId="59" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="217.5" dataDxfId="58" totalsRowDxfId="57"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="56" totalsRowDxfId="55">
-      <totalsRowFormula>"M666 X-"&amp;N25&amp;" Y-"&amp;N26&amp;" Z-"&amp;N27</totalsRowFormula>
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="11"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="10"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="9"/>
+    <tableColumn id="6" name="Z" dataDxfId="87" totalsRowDxfId="8" dataCellStyle="Comma"/>
+    <tableColumn id="7" name=" " dataDxfId="86" totalsRowDxfId="7"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="85" totalsRowDxfId="6">
+      <totalsRowFormula>"M666 X-"&amp;ROUND(N25,2)&amp;" Y-"&amp;ROUND(N26,2)&amp;" Z-"&amp;ROUND(N27,2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
@@ -3444,12 +4011,12 @@
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B6:G12" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="54"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="53"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="52"/>
-    <tableColumn id="6" name="Z" dataDxfId="51" totalsRowDxfId="50" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="215.5" dataDxfId="49" totalsRowDxfId="48"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="47" totalsRowDxfId="46">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="84"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="83"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="82"/>
+    <tableColumn id="6" name="Z" dataDxfId="81" totalsRowDxfId="80" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="215.5" dataDxfId="79" totalsRowDxfId="78"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="77" totalsRowDxfId="76">
       <totalsRowFormula>"M666 X-"&amp;G9&amp;" Y-"&amp;G10&amp;" Z-"&amp;G11</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3460,12 +4027,12 @@
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1425" displayName="Table1425" ref="B14:G20" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="45"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="44"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="43"/>
-    <tableColumn id="6" name="Z" dataDxfId="42" totalsRowDxfId="41" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="216.5" dataDxfId="40" totalsRowDxfId="39"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="38" totalsRowDxfId="37">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="75"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="74"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="73"/>
+    <tableColumn id="6" name="Z" dataDxfId="72" totalsRowDxfId="71" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="216.5" dataDxfId="70" totalsRowDxfId="69"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="68" totalsRowDxfId="67">
       <totalsRowFormula>"M666 X-"&amp;G17&amp;" Y-"&amp;G18&amp;" Z-"&amp;G19</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3476,12 +4043,12 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1427" displayName="Table1427" ref="I6:N12" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="36"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="35"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="34"/>
-    <tableColumn id="6" name="Z" dataDxfId="33" totalsRowDxfId="32" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="216.0" dataDxfId="31" totalsRowDxfId="30"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="29" totalsRowDxfId="28">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="66"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="65"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="64"/>
+    <tableColumn id="6" name="Z" dataDxfId="63" totalsRowDxfId="62" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="216.0" dataDxfId="61" totalsRowDxfId="60"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="59" totalsRowDxfId="58">
       <totalsRowFormula>"M666 X-"&amp;N9&amp;" Y-"&amp;N10&amp;" Z-"&amp;N11</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3813,8 +4380,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N28"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3835,14 +4402,14 @@
       </c>
       <c r="C1" s="3" t="str">
         <f>Parameters!E9</f>
-        <v>G0 X0 Y0 Z10 E0</v>
+        <v>G0 X0 Y0 Z50 E0</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>33</v>
       </c>
       <c r="J1" s="3" t="str">
         <f>Parameters!E9</f>
-        <v>G0 X0 Y0 Z10 E0</v>
+        <v>G0 X0 Y0 Z50 E0</v>
       </c>
     </row>
     <row r="2" spans="2:14">
@@ -3851,14 +4418,14 @@
       </c>
       <c r="C2" s="3" t="str">
         <f>Parameters!E11</f>
-        <v>G0 X-99.46 Y-57.43 Z10 E0</v>
+        <v>G0 X-99.46 Y-57.43 Z50 E0</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>2</v>
       </c>
       <c r="J2" s="3" t="str">
         <f>Parameters!E11</f>
-        <v>G0 X-99.46 Y-57.43 Z10 E0</v>
+        <v>G0 X-99.46 Y-57.43 Z50 E0</v>
       </c>
     </row>
     <row r="3" spans="2:14">
@@ -3867,14 +4434,14 @@
       </c>
       <c r="C3" s="3" t="str">
         <f>Parameters!E13</f>
-        <v>G0 X99.46 Y-57.43 Z10 E0</v>
+        <v>G0 X99.46 Y-57.43 Z50 E0</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="3" t="str">
         <f>Parameters!E13</f>
-        <v>G0 X99.46 Y-57.43 Z10 E0</v>
+        <v>G0 X99.46 Y-57.43 Z50 E0</v>
       </c>
     </row>
     <row r="4" spans="2:14">
@@ -3883,14 +4450,14 @@
       </c>
       <c r="C4" s="3" t="str">
         <f>Parameters!E15</f>
-        <v>G0 X0 Y114.85 Z10 E0</v>
+        <v>G0 X0 Y114.85 Z50 E0</v>
       </c>
       <c r="I4" s="15" t="s">
         <v>4</v>
       </c>
       <c r="J4" s="3" t="str">
         <f>Parameters!E15</f>
-        <v>G0 X0 Y114.85 Z10 E0</v>
+        <v>G0 X0 Y114.85 Z50 E0</v>
       </c>
     </row>
     <row r="6" spans="2:14">
@@ -3925,7 +4492,7 @@
         <v>4</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>34</v>
+        <v>68</v>
       </c>
       <c r="N6" s="1" t="s">
         <v>27</v>
@@ -3943,7 +4510,7 @@
       </c>
       <c r="G7" s="6">
         <f>MIN(F9:F11)</f>
-        <v>120</v>
+        <v>113.4</v>
       </c>
       <c r="I7" t="s">
         <v>5</v>
@@ -3968,11 +4535,11 @@
         <v>0</v>
       </c>
       <c r="E8" s="5">
-        <v>6.3</v>
+        <v>6.7</v>
       </c>
       <c r="F8" s="6">
         <f>F$7-Table146[[#This Row],[Z]]</f>
-        <v>113.7</v>
+        <v>113.3</v>
       </c>
       <c r="G8"/>
       <c r="I8" t="s">
@@ -4001,14 +4568,16 @@
       <c r="D9" s="5">
         <v>-57.4</v>
       </c>
-      <c r="E9" s="5"/>
+      <c r="E9" s="5">
+        <v>6.5</v>
+      </c>
       <c r="F9" s="6">
         <f>F$7-Table146[[#This Row],[Z]]</f>
-        <v>120</v>
+        <v>113.5</v>
       </c>
       <c r="G9" s="6">
         <f>ROUNDUP(MAX(E$9:E$11),1)-Table146[[#This Row],[Z]]</f>
-        <v>0</v>
+        <v>9.9999999999999645E-2</v>
       </c>
       <c r="I9" t="s">
         <v>7</v>
@@ -4039,13 +4608,15 @@
       <c r="D10" s="5">
         <v>-57.4</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="5">
+        <v>6.6</v>
+      </c>
       <c r="F10" s="6">
         <f>F$7-Table146[[#This Row],[Z]]</f>
-        <v>120</v>
+        <v>113.4</v>
       </c>
       <c r="G10" s="6">
-        <f>ROUNDUP(MAX(E$17:E$19),1)-Table146[[#This Row],[Z]]</f>
+        <f>ROUNDUP(MAX(E$9:E$11),1)-Table146[[#This Row],[Z]]</f>
         <v>0</v>
       </c>
       <c r="I10" t="s">
@@ -4077,14 +4648,16 @@
       <c r="D11" s="5">
         <v>114.8</v>
       </c>
-      <c r="E11" s="5"/>
+      <c r="E11" s="5">
+        <v>6.5</v>
+      </c>
       <c r="F11" s="6">
         <f>F$7-Table146[[#This Row],[Z]]</f>
-        <v>120</v>
+        <v>113.5</v>
       </c>
       <c r="G11" s="6">
-        <f>ROUNDUP(MAX(E$17:E$19),1)-Table146[[#This Row],[Z]]</f>
-        <v>0</v>
+        <f>ROUNDUP(MAX(E$9:E$11),1)-Table146[[#This Row],[Z]]</f>
+        <v>9.9999999999999645E-2</v>
       </c>
       <c r="I11" t="s">
         <v>9</v>
@@ -4112,8 +4685,8 @@
       <c r="E12" s="16"/>
       <c r="F12" s="13"/>
       <c r="G12" s="14" t="str">
-        <f>"M666 X-"&amp;G9&amp;" Y-"&amp;G10&amp;" Z-"&amp;G11</f>
-        <v>M666 X-0 Y-0 Z-0</v>
+        <f>"M666 X-"&amp;ROUND(G9,2)&amp;" Y-"&amp;ROUND(G10,2)&amp;" Z-"&amp;ROUND(G11,2)</f>
+        <v>M666 X-0.1 Y-0 Z-0.1</v>
       </c>
       <c r="I12" s="12"/>
       <c r="J12" s="12"/>
@@ -4121,7 +4694,7 @@
       <c r="L12" s="16"/>
       <c r="M12" s="13"/>
       <c r="N12" s="14" t="str">
-        <f>"M666 X-"&amp;N9&amp;" Y-"&amp;N10&amp;" Z-"&amp;N11</f>
+        <f>"M666 X-"&amp;ROUND(N9,2)&amp;" Y-"&amp;ROUND(N10,2)&amp;" Z-"&amp;ROUND(N11,2)</f>
         <v>M666 X-0 Y-0 Z-0</v>
       </c>
     </row>
@@ -4139,7 +4712,7 @@
         <v>4</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>27</v>
@@ -4157,7 +4730,7 @@
         <v>4</v>
       </c>
       <c r="M14" s="11" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="N14" s="1" t="s">
         <v>27</v>
@@ -4170,10 +4743,12 @@
       <c r="C15" s="4"/>
       <c r="D15" s="4"/>
       <c r="E15" s="4"/>
-      <c r="F15" s="6"/>
+      <c r="F15" s="6">
+        <v>120</v>
+      </c>
       <c r="G15" s="6">
         <f>MIN(F17:F19)</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="I15" t="s">
         <v>5</v>
@@ -4200,7 +4775,7 @@
       <c r="E16" s="5"/>
       <c r="F16" s="6">
         <f>F$15-Table142510[[#This Row],[Z]]</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G16"/>
       <c r="I16" t="s">
@@ -4232,7 +4807,7 @@
       <c r="E17" s="5"/>
       <c r="F17" s="6">
         <f>F$15-Table142510[[#This Row],[Z]]</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G17" s="6">
         <f>ROUNDUP(MAX(E$17:E$19),1)-Table142510[[#This Row],[Z]]</f>
@@ -4270,7 +4845,7 @@
       <c r="E18" s="5"/>
       <c r="F18" s="6">
         <f>F$15-Table142510[[#This Row],[Z]]</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G18" s="6">
         <f>ROUNDUP(MAX(E$17:E$19),1)-Table142510[[#This Row],[Z]]</f>
@@ -4308,7 +4883,7 @@
       <c r="E19" s="5"/>
       <c r="F19" s="6">
         <f>F$15-Table142510[[#This Row],[Z]]</f>
-        <v>0</v>
+        <v>120</v>
       </c>
       <c r="G19" s="6">
         <f>ROUNDUP(MAX(E$17:E$19),1)-Table142510[[#This Row],[Z]]</f>
@@ -4340,7 +4915,7 @@
       <c r="E20" s="16"/>
       <c r="F20" s="13"/>
       <c r="G20" s="14" t="str">
-        <f>"M666 X-"&amp;G17&amp;" Y-"&amp;G18&amp;" Z-"&amp;G19</f>
+        <f>"M666 X-"&amp;ROUND(G17,2)&amp;" Y-"&amp;ROUND(G18,2)&amp;" Z-"&amp;ROUND(G19,2)</f>
         <v>M666 X-0 Y-0 Z-0</v>
       </c>
       <c r="I20" s="12"/>
@@ -4349,7 +4924,7 @@
       <c r="L20" s="16"/>
       <c r="M20" s="13"/>
       <c r="N20" s="14" t="str">
-        <f>"M666 X-"&amp;N17&amp;" Y-"&amp;N18&amp;" Z-"&amp;N19</f>
+        <f>"M666 X-"&amp;ROUND(N17,2)&amp;" Y-"&amp;ROUND(N18,2)&amp;" Z-"&amp;ROUND(N19,2)</f>
         <v>M666 X-0 Y-0 Z-0</v>
       </c>
     </row>
@@ -4367,7 +4942,7 @@
         <v>4</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="G22" s="1" t="s">
         <v>27</v>
@@ -4385,7 +4960,7 @@
         <v>4</v>
       </c>
       <c r="M22" s="11" t="s">
-        <v>37</v>
+        <v>68</v>
       </c>
       <c r="N22" s="1" t="s">
         <v>27</v>
@@ -4463,7 +5038,7 @@
         <v>0</v>
       </c>
       <c r="G25" s="6">
-        <f>MAX(E$25:E$27)-Table14258913[[#This Row],[Z]]</f>
+        <f>ROUNDUP(MAX(E$25:E$27),1)-Table14258913[[#This Row],[Z]]</f>
         <v>0</v>
       </c>
       <c r="I25" t="s">
@@ -4481,7 +5056,7 @@
         <v>0</v>
       </c>
       <c r="N25" s="6">
-        <f>MAX(L$25:L$27)-Table142589214[[#This Row],[Z]]</f>
+        <f>ROUNDUP(MAX(L$25:L$27),1)-Table14258913[[#This Row],[Z]]</f>
         <v>0</v>
       </c>
     </row>
@@ -4501,7 +5076,7 @@
         <v>0</v>
       </c>
       <c r="G26" s="6">
-        <f>MAX(E$25:E$27)-Table14258913[[#This Row],[Z]]</f>
+        <f>ROUNDUP(MAX(E$25:E$27),1)-Table14258913[[#This Row],[Z]]</f>
         <v>0</v>
       </c>
       <c r="I26" t="s">
@@ -4519,7 +5094,7 @@
         <v>0</v>
       </c>
       <c r="N26" s="6">
-        <f>MAX(L$25:L$27)-Table142589214[[#This Row],[Z]]</f>
+        <f>ROUNDUP(MAX(L$25:L$27),1)-Table14258913[[#This Row],[Z]]</f>
         <v>0</v>
       </c>
     </row>
@@ -4539,7 +5114,7 @@
         <v>0</v>
       </c>
       <c r="G27" s="6">
-        <f>MAX(E$25:E$27)-Table14258913[[#This Row],[Z]]</f>
+        <f>ROUNDUP(MAX(E$25:E$27),1)-Table14258913[[#This Row],[Z]]</f>
         <v>0</v>
       </c>
       <c r="I27" t="s">
@@ -4557,7 +5132,7 @@
         <v>0</v>
       </c>
       <c r="N27" s="6">
-        <f>MAX(L$25:L$27)-Table142589214[[#This Row],[Z]]</f>
+        <f>ROUNDUP(MAX(L$25:L$27),1)-Table14258913[[#This Row],[Z]]</f>
         <v>0</v>
       </c>
     </row>
@@ -4568,7 +5143,7 @@
       <c r="E28" s="16"/>
       <c r="F28" s="13"/>
       <c r="G28" s="14" t="str">
-        <f>"M666 X-"&amp;G25&amp;" Y-"&amp;G26&amp;" Z-"&amp;G27</f>
+        <f>"M666 X-"&amp;ROUND(G25,2)&amp;" Y-"&amp;ROUND(G26,2)&amp;" Z-"&amp;ROUND(G27,2)</f>
         <v>M666 X-0 Y-0 Z-0</v>
       </c>
       <c r="I28" s="12"/>
@@ -4577,7 +5152,7 @@
       <c r="L28" s="16"/>
       <c r="M28" s="13"/>
       <c r="N28" s="14" t="str">
-        <f>"M666 X-"&amp;N25&amp;" Y-"&amp;N26&amp;" Z-"&amp;N27</f>
+        <f>"M666 X-"&amp;ROUND(N25,2)&amp;" Y-"&amp;ROUND(N26,2)&amp;" Z-"&amp;ROUND(N27,2)</f>
         <v>M666 X-0 Y-0 Z-0</v>
       </c>
     </row>
@@ -4627,14 +5202,14 @@
       </c>
       <c r="C1" s="3" t="str">
         <f>Parameters!E9</f>
-        <v>G0 X0 Y0 Z10 E0</v>
+        <v>G0 X0 Y0 Z50 E0</v>
       </c>
       <c r="I1" s="15" t="s">
         <v>33</v>
       </c>
       <c r="J1" s="3" t="str">
         <f>Parameters!E9</f>
-        <v>G0 X0 Y0 Z10 E0</v>
+        <v>G0 X0 Y0 Z50 E0</v>
       </c>
     </row>
     <row r="2" spans="2:14">
@@ -4643,14 +5218,14 @@
       </c>
       <c r="C2" s="3" t="str">
         <f>Parameters!E11</f>
-        <v>G0 X-99.46 Y-57.43 Z10 E0</v>
+        <v>G0 X-99.46 Y-57.43 Z50 E0</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>2</v>
       </c>
       <c r="J2" s="3" t="str">
         <f>Parameters!E11</f>
-        <v>G0 X-99.46 Y-57.43 Z10 E0</v>
+        <v>G0 X-99.46 Y-57.43 Z50 E0</v>
       </c>
     </row>
     <row r="3" spans="2:14">
@@ -4659,14 +5234,14 @@
       </c>
       <c r="C3" s="3" t="str">
         <f>Parameters!E13</f>
-        <v>G0 X99.46 Y-57.43 Z10 E0</v>
+        <v>G0 X99.46 Y-57.43 Z50 E0</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>3</v>
       </c>
       <c r="J3" s="3" t="str">
         <f>Parameters!E13</f>
-        <v>G0 X99.46 Y-57.43 Z10 E0</v>
+        <v>G0 X99.46 Y-57.43 Z50 E0</v>
       </c>
     </row>
     <row r="4" spans="2:14">
@@ -4675,14 +5250,14 @@
       </c>
       <c r="C4" s="3" t="str">
         <f>Parameters!E15</f>
-        <v>G0 X0 Y114.85 Z10 E0</v>
+        <v>G0 X0 Y114.85 Z50 E0</v>
       </c>
       <c r="I4" s="15" t="s">
         <v>4</v>
       </c>
       <c r="J4" s="3" t="str">
         <f>Parameters!E15</f>
-        <v>G0 X0 Y114.85 Z10 E0</v>
+        <v>G0 X0 Y114.85 Z50 E0</v>
       </c>
     </row>
     <row r="6" spans="2:14">
@@ -5403,8 +5978,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:H32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5454,7 +6029,7 @@
       </c>
       <c r="C8" s="18" t="str">
         <f>Parameters!E9</f>
-        <v>G0 X0 Y0 Z10 E0</v>
+        <v>G0 X0 Y0 Z50 E0</v>
       </c>
     </row>
     <row r="9" spans="1:8">
@@ -5463,7 +6038,7 @@
       </c>
       <c r="C9" s="18" t="str">
         <f>Parameters!E11</f>
-        <v>G0 X-99.46 Y-57.43 Z10 E0</v>
+        <v>G0 X-99.46 Y-57.43 Z50 E0</v>
       </c>
     </row>
     <row r="10" spans="1:8">
@@ -5472,7 +6047,7 @@
       </c>
       <c r="C10" s="18" t="str">
         <f>Parameters!E13</f>
-        <v>G0 X99.46 Y-57.43 Z10 E0</v>
+        <v>G0 X99.46 Y-57.43 Z50 E0</v>
       </c>
     </row>
     <row r="11" spans="1:8">
@@ -5481,7 +6056,7 @@
       </c>
       <c r="C11" s="18" t="str">
         <f>Parameters!E15</f>
-        <v>G0 X0 Y114.85 Z10 E0</v>
+        <v>G0 X0 Y114.85 Z50 E0</v>
       </c>
     </row>
     <row r="13" spans="1:8">
@@ -5607,7 +6182,7 @@
   <dimension ref="B2:E23"/>
   <sheetViews>
     <sheetView showGridLines="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5666,6 +6241,12 @@
       <c r="C7" s="9">
         <v>17</v>
       </c>
+      <c r="D7" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
     </row>
     <row r="8" spans="2:5">
       <c r="B8" s="7" t="s">
@@ -5687,8 +6268,8 @@
         <v>33</v>
       </c>
       <c r="E9" t="str">
-        <f>"G0 X0 Y0 Z10 E0"</f>
-        <v>G0 X0 Y0 Z10 E0</v>
+        <f>"G0 X0 Y0 Z"&amp;Height&amp;" E0"</f>
+        <v>G0 X0 Y0 Z50 E0</v>
       </c>
     </row>
     <row r="10" spans="2:5">
@@ -5711,8 +6292,8 @@
         <v>2</v>
       </c>
       <c r="E11" t="str">
-        <f>"G0 X"&amp;DELTA_TOWER1_X&amp;" Y"&amp;DELTA_TOWER1_Y&amp;" Z10 E0"</f>
-        <v>G0 X-99.46 Y-57.43 Z10 E0</v>
+        <f>"G0 X"&amp;DELTA_TOWER1_X&amp;" Y"&amp;DELTA_TOWER1_Y&amp;" Z"&amp;Height&amp;" E0"</f>
+        <v>G0 X-99.46 Y-57.43 Z50 E0</v>
       </c>
     </row>
     <row r="12" spans="2:5">
@@ -5737,8 +6318,8 @@
         <v>3</v>
       </c>
       <c r="E13" t="str">
-        <f>"G0 X"&amp;DELTA_TOWER3_X&amp;" Y"&amp;DELTA_TOWER3_Y&amp;" Z10 E0"</f>
-        <v>G0 X99.46 Y-57.43 Z10 E0</v>
+        <f>"G0 X"&amp;DELTA_TOWER3_X&amp;" Y"&amp;DELTA_TOWER3_Y&amp;" Z"&amp;Height&amp;" E0"</f>
+        <v>G0 X99.46 Y-57.43 Z50 E0</v>
       </c>
     </row>
     <row r="14" spans="2:5">
@@ -5762,8 +6343,8 @@
         <v>4</v>
       </c>
       <c r="E15" t="str">
-        <f>"G0 X"&amp;DELTA_TOWER2_X&amp;" Y"&amp;DELTA_TOWER2_Y&amp;" Z10 E0"</f>
-        <v>G0 X0 Y114.85 Z10 E0</v>
+        <f>"G0 X"&amp;DELTA_TOWER2_X&amp;" Y"&amp;DELTA_TOWER2_Y&amp;" Z"&amp;Height&amp;" E0"</f>
+        <v>G0 X0 Y114.85 Z50 E0</v>
       </c>
     </row>
     <row r="16" spans="2:5">

</xml_diff>

<commit_message>
Adjusted to 113.5 for bed level
</commit_message>
<xml_diff>
--- a/Marlin/3DR Calibration.xlsx
+++ b/Marlin/3DR Calibration.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25306"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19180" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="19440" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Positions - Heated" sheetId="4" r:id="rId1"/>
@@ -818,9 +818,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="786">
+  <cellStyleXfs count="792">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1641,7 +1647,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="786">
+  <cellStyles count="792">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Followed Hyperlink" xfId="3" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="5" builtinId="9" hidden="1"/>
@@ -2035,6 +2041,9 @@
     <cellStyle name="Followed Hyperlink" xfId="781" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="783" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="785" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="787" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="789" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="791" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="2" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="4" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="6" builtinId="8" hidden="1"/>
@@ -2427,6 +2436,9 @@
     <cellStyle name="Hyperlink" xfId="780" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="782" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="784" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="786" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="788" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="790" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="109">
@@ -2534,6 +2546,9 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
       <fill>
         <patternFill patternType="solid">
@@ -2551,18 +2566,24 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -2595,6 +2616,15 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2654,18 +2684,24 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -2698,6 +2734,15 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2757,18 +2802,24 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -2801,6 +2852,15 @@
       </border>
     </dxf>
     <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -2860,18 +2920,24 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
     </dxf>
     <dxf>
       <font>
@@ -2904,49 +2970,55 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
@@ -3540,6 +3612,21 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.0"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -3655,81 +3742,6 @@
         <top/>
         <bottom/>
       </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="165" formatCode="0.0"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <numFmt numFmtId="165" formatCode="0.0"/>
@@ -3873,12 +3885,12 @@
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="7" name="Table14258" displayName="Table14258" ref="I14:N20" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="57"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="56"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="55"/>
-    <tableColumn id="6" name="Z" dataDxfId="54" totalsRowDxfId="53" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="217.0" dataDxfId="52" totalsRowDxfId="51"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="50" totalsRowDxfId="49">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="33"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="32"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="31"/>
+    <tableColumn id="6" name="Z" dataDxfId="30" totalsRowDxfId="29" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="217.0" dataDxfId="28" totalsRowDxfId="27"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="26" totalsRowDxfId="25">
       <totalsRowFormula>"M666 X-"&amp;N17&amp;" Y-"&amp;N18&amp;" Z-"&amp;N19</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3889,12 +3901,12 @@
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="8" name="Table142589" displayName="Table142589" ref="B22:G28" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="48"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="47"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="46"/>
-    <tableColumn id="6" name="Z" dataDxfId="45" totalsRowDxfId="44" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="217.5" dataDxfId="43" totalsRowDxfId="42"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="41" totalsRowDxfId="40">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="24"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="23"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="22"/>
+    <tableColumn id="6" name="Z" dataDxfId="21" totalsRowDxfId="20" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="217.5" dataDxfId="19" totalsRowDxfId="18"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="17" totalsRowDxfId="16">
       <totalsRowFormula>"M666 X-"&amp;G25&amp;" Y-"&amp;G26&amp;" Z-"&amp;G27</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3905,12 +3917,12 @@
 <file path=xl/tables/table12.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1425892" displayName="Table1425892" ref="I22:N28" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="39"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="38"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="37"/>
-    <tableColumn id="6" name="Z" dataDxfId="36" totalsRowDxfId="35" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="217.5" dataDxfId="34" totalsRowDxfId="33"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="32" totalsRowDxfId="31">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="15"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="14"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="13"/>
+    <tableColumn id="6" name="Z" dataDxfId="12" totalsRowDxfId="11" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="217.5" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="8" totalsRowDxfId="7">
       <totalsRowFormula>"M666 X-"&amp;N25&amp;" Y-"&amp;N26&amp;" Z-"&amp;N27</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3922,7 +3934,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B2:C16" totalsRowShown="0">
   <tableColumns count="2">
     <tableColumn id="1" name="Parameter"/>
-    <tableColumn id="2" name="Value" dataDxfId="30"/>
+    <tableColumn id="2" name="Value" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="1"/>
 </table>
@@ -3931,12 +3943,12 @@
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="9" name="Table142510" displayName="Table142510" ref="B14:G20" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="23"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="22"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="21"/>
-    <tableColumn id="6" name="Z" dataDxfId="99" totalsRowDxfId="20" dataCellStyle="Comma"/>
-    <tableColumn id="7" name=" " dataDxfId="98" totalsRowDxfId="19"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="97" totalsRowDxfId="18">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="99"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="98"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="97"/>
+    <tableColumn id="6" name="Z" dataDxfId="96" totalsRowDxfId="95" dataCellStyle="Comma"/>
+    <tableColumn id="7" name=" " dataDxfId="94" totalsRowDxfId="93"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="92" totalsRowDxfId="91">
       <totalsRowFormula>"M666 X-"&amp;ROUND(G17,2)&amp;" Y-"&amp;ROUND(G18,2)&amp;" Z-"&amp;ROUND(G19,2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3950,9 +3962,9 @@
     <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="5"/>
     <tableColumn id="3" name="X" totalsRowDxfId="4"/>
     <tableColumn id="4" name="Y" totalsRowDxfId="3"/>
-    <tableColumn id="6" name="Z" dataDxfId="96" totalsRowDxfId="2" dataCellStyle="Comma"/>
-    <tableColumn id="7" name=" " dataDxfId="95" totalsRowDxfId="1"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="94" totalsRowDxfId="0">
+    <tableColumn id="6" name="Z" dataDxfId="90" totalsRowDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="7" name=" " dataDxfId="89" totalsRowDxfId="1"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="88" totalsRowDxfId="0">
       <totalsRowFormula>"M666 X-"&amp;ROUND(N9,2)&amp;" Y-"&amp;ROUND(N10,2)&amp;" Z-"&amp;ROUND(N11,2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3963,12 +3975,12 @@
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="11" name="Table1425812" displayName="Table1425812" ref="I14:N20" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="29"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="28"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="27"/>
-    <tableColumn id="6" name="Z" dataDxfId="93" totalsRowDxfId="26" dataCellStyle="Comma"/>
-    <tableColumn id="7" name=" " dataDxfId="92" totalsRowDxfId="25"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="91" totalsRowDxfId="24">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="87"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="86"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="85"/>
+    <tableColumn id="6" name="Z" dataDxfId="84" totalsRowDxfId="83" dataCellStyle="Comma"/>
+    <tableColumn id="7" name=" " dataDxfId="82" totalsRowDxfId="81"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="80" totalsRowDxfId="79">
       <totalsRowFormula>"M666 X-"&amp;ROUND(N17,2)&amp;" Y-"&amp;ROUND(N18,2)&amp;" Z-"&amp;ROUND(N19,2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3979,12 +3991,12 @@
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="12" name="Table14258913" displayName="Table14258913" ref="B22:G28" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="17"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="16"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="15"/>
-    <tableColumn id="6" name="Z" dataDxfId="90" totalsRowDxfId="14" dataCellStyle="Comma"/>
-    <tableColumn id="7" name=" " dataDxfId="89" totalsRowDxfId="13"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="88" totalsRowDxfId="12">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="78"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="77"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="76"/>
+    <tableColumn id="6" name="Z" dataDxfId="75" totalsRowDxfId="74" dataCellStyle="Comma"/>
+    <tableColumn id="7" name=" " dataDxfId="73" totalsRowDxfId="72"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="71" totalsRowDxfId="70">
       <totalsRowFormula>"M666 X-"&amp;ROUND(G25,2)&amp;" Y-"&amp;ROUND(G26,2)&amp;" Z-"&amp;ROUND(G27,2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -3995,12 +4007,12 @@
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="13" name="Table142589214" displayName="Table142589214" ref="I22:N28" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="11"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="10"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="9"/>
-    <tableColumn id="6" name="Z" dataDxfId="87" totalsRowDxfId="8" dataCellStyle="Comma"/>
-    <tableColumn id="7" name=" " dataDxfId="86" totalsRowDxfId="7"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="85" totalsRowDxfId="6">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="69"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="68"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="67"/>
+    <tableColumn id="6" name="Z" dataDxfId="66" totalsRowDxfId="65" dataCellStyle="Comma"/>
+    <tableColumn id="7" name=" " dataDxfId="64" totalsRowDxfId="63"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="62" totalsRowDxfId="61">
       <totalsRowFormula>"M666 X-"&amp;ROUND(N25,2)&amp;" Y-"&amp;ROUND(N26,2)&amp;" Z-"&amp;ROUND(N27,2)</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -4011,12 +4023,12 @@
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table14" displayName="Table14" ref="B6:G12" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="84"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="83"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="82"/>
-    <tableColumn id="6" name="Z" dataDxfId="81" totalsRowDxfId="80" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="215.5" dataDxfId="79" totalsRowDxfId="78"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="77" totalsRowDxfId="76">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="60"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="59"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="58"/>
+    <tableColumn id="6" name="Z" dataDxfId="57" totalsRowDxfId="56" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="215.5" dataDxfId="55" totalsRowDxfId="54"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="53" totalsRowDxfId="52">
       <totalsRowFormula>"M666 X-"&amp;G9&amp;" Y-"&amp;G10&amp;" Z-"&amp;G11</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -4027,12 +4039,12 @@
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table1425" displayName="Table1425" ref="B14:G20" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="75"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="74"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="73"/>
-    <tableColumn id="6" name="Z" dataDxfId="72" totalsRowDxfId="71" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="216.5" dataDxfId="70" totalsRowDxfId="69"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="68" totalsRowDxfId="67">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="51"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="50"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="49"/>
+    <tableColumn id="6" name="Z" dataDxfId="48" totalsRowDxfId="47" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="216.5" dataDxfId="46" totalsRowDxfId="45"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="44" totalsRowDxfId="43">
       <totalsRowFormula>"M666 X-"&amp;G17&amp;" Y-"&amp;G18&amp;" Z-"&amp;G19</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -4043,12 +4055,12 @@
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table1427" displayName="Table1427" ref="I6:N12" totalsRowCount="1">
   <tableColumns count="6">
-    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="66"/>
-    <tableColumn id="3" name="X" totalsRowDxfId="65"/>
-    <tableColumn id="4" name="Y" totalsRowDxfId="64"/>
-    <tableColumn id="6" name="Z" dataDxfId="63" totalsRowDxfId="62" dataCellStyle="Comma"/>
-    <tableColumn id="7" name="216.0" dataDxfId="61" totalsRowDxfId="60"/>
-    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="59" totalsRowDxfId="58">
+    <tableColumn id="1" name="DELTA_DIAGONAL_ROD" totalsRowDxfId="42"/>
+    <tableColumn id="3" name="X" totalsRowDxfId="41"/>
+    <tableColumn id="4" name="Y" totalsRowDxfId="40"/>
+    <tableColumn id="6" name="Z" dataDxfId="39" totalsRowDxfId="38" dataCellStyle="Comma"/>
+    <tableColumn id="7" name="216.0" dataDxfId="37" totalsRowDxfId="36"/>
+    <tableColumn id="8" name="Offset" totalsRowFunction="custom" dataDxfId="35" totalsRowDxfId="34">
       <totalsRowFormula>"M666 X-"&amp;N9&amp;" Y-"&amp;N10&amp;" Z-"&amp;N11</totalsRowFormula>
     </tableColumn>
   </tableColumns>
@@ -4381,7 +4393,7 @@
   <dimension ref="B1:N28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -4518,10 +4530,12 @@
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
       <c r="L7" s="4"/>
-      <c r="M7" s="6"/>
+      <c r="M7" s="6">
+        <v>113.4</v>
+      </c>
       <c r="N7" s="6">
         <f>MIN(M9:M11)</f>
-        <v>0</v>
+        <v>113.4</v>
       </c>
     </row>
     <row r="8" spans="2:14">
@@ -4554,7 +4568,7 @@
       <c r="L8" s="5"/>
       <c r="M8" s="6">
         <f>M$7-Table142711[[#This Row],[Z]]</f>
-        <v>0</v>
+        <v>113.4</v>
       </c>
       <c r="N8"/>
     </row>
@@ -4591,7 +4605,7 @@
       <c r="L9" s="5"/>
       <c r="M9" s="6">
         <f>M$7-Table142711[[#This Row],[Z]]</f>
-        <v>0</v>
+        <v>113.4</v>
       </c>
       <c r="N9" s="6">
         <f>ROUNDUP(MAX(L$9:L$11),1)-Table142711[[#This Row],[Z]]</f>
@@ -4631,7 +4645,7 @@
       <c r="L10" s="5"/>
       <c r="M10" s="6">
         <f>M$7-Table142711[[#This Row],[Z]]</f>
-        <v>0</v>
+        <v>113.4</v>
       </c>
       <c r="N10" s="6">
         <f>ROUNDUP(MAX(L$9:L$11),1)-Table142711[[#This Row],[Z]]</f>
@@ -4671,7 +4685,7 @@
       <c r="L11" s="5"/>
       <c r="M11" s="6">
         <f>M$7-Table142711[[#This Row],[Z]]</f>
-        <v>0</v>
+        <v>113.4</v>
       </c>
       <c r="N11" s="6">
         <f>ROUNDUP(MAX(L$9:L$11),1)-Table142711[[#This Row],[Z]]</f>

</xml_diff>